<commit_message>
updated what to writre
</commit_message>
<xml_diff>
--- a/code to write.xlsx
+++ b/code to write.xlsx
@@ -105,12 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -431,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -442,92 +441,80 @@
     <col min="1" max="1" width="74.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>